<commit_message>
fixes: add extra dists and TODO
</commit_message>
<xml_diff>
--- a/calculator.xlsx
+++ b/calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikejseay\Documents\Code\retirement\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D421DE9-B667-4C89-928E-F485E0A44EDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27BD7258-0E76-4C4D-9EEE-39ADE39FCB39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="comments" sheetId="3" r:id="rId1"/>
@@ -273,7 +273,7 @@
     <numFmt numFmtId="164" formatCode="\$#,##0_);\(\$#,##0\)"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000%"/>
     <numFmt numFmtId="166" formatCode="#,##0%"/>
-    <numFmt numFmtId="168" formatCode="0.0%"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -315,7 +315,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -325,6 +325,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -350,141 +356,141 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="7" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="7" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="4" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -495,6 +501,12 @@
     </xf>
     <xf numFmtId="3" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -803,7 +815,7 @@
   <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,7 +868,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,7 +1028,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,7 +1085,7 @@
         <v>11925</v>
       </c>
       <c r="F3" s="6">
-        <f>IF(  E3&gt;0,E3*D3,0)</f>
+        <f t="shared" ref="F3:F8" si="0">IF(  E3&gt;0,E3*D3,0)</f>
         <v>1192.5</v>
       </c>
       <c r="G3" s="6">
@@ -1099,7 +1111,7 @@
         <v>36550</v>
       </c>
       <c r="F4" s="6">
-        <f>IF(  E4&gt;0,E4*D4,0)</f>
+        <f t="shared" si="0"/>
         <v>4386</v>
       </c>
       <c r="G4" s="6">
@@ -1122,7 +1134,7 @@
         <v>29260</v>
       </c>
       <c r="F5" s="6">
-        <f>IF(  E5&gt;0,E5*D5,0)</f>
+        <f t="shared" si="0"/>
         <v>6437.2</v>
       </c>
       <c r="G5" s="6">
@@ -1145,7 +1157,7 @@
         <v>0</v>
       </c>
       <c r="F6" s="6">
-        <f>IF(  E6&gt;0,E6*D6,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G6" s="6">
@@ -1168,7 +1180,7 @@
         <v>0</v>
       </c>
       <c r="F7" s="6">
-        <f>IF(  E7&gt;0,E7*D7,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G7" s="6">
@@ -1191,7 +1203,7 @@
         <v>0</v>
       </c>
       <c r="F8" s="6">
-        <f>IF(  E8&gt;0,E8*D8,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="G8" s="6">
@@ -1224,7 +1236,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1329,14 +1341,14 @@
   </sheetPr>
   <dimension ref="A1:AD788"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E3" sqref="E3"/>
+      <selection pane="topRight" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" style="31" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.42578125" style="31" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.28515625" style="32" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" style="31" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.42578125" style="32" bestFit="1" customWidth="1"/>
@@ -1354,8 +1366,8 @@
     <col min="16" max="16" width="17" style="32" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="18" style="32" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="16.140625" style="32" bestFit="1" customWidth="1"/>
-    <col min="19" max="21" width="11.5703125" style="32" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="6.140625" style="32" bestFit="1" customWidth="1"/>
+    <col min="19" max="21" width="12.28515625" style="32" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="6.28515625" style="32" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="18.5703125" style="32"/>
     <col min="25" max="25" width="13.42578125" style="32" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="17" style="32" bestFit="1" customWidth="1"/>
@@ -1446,13 +1458,13 @@
       <c r="C2" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="49" t="s">
         <v>47</v>
       </c>
       <c r="G2" s="25" t="s">
@@ -1485,7 +1497,7 @@
       <c r="P2" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="Q2" s="16" t="s">
+      <c r="Q2" s="50" t="s">
         <v>59</v>
       </c>
       <c r="R2" s="29">
@@ -1742,7 +1754,7 @@
         <v>5000</v>
       </c>
       <c r="D5" s="6">
-        <f>D4+K4-J4-B4</f>
+        <f t="shared" ref="D5:D18" si="4">D4+K4-J4-B4</f>
         <v>1096241.7842400002</v>
       </c>
       <c r="E5" s="6">
@@ -1754,18 +1766,18 @@
         <v>11324.691791775113</v>
       </c>
       <c r="G5" s="22">
-        <f t="shared" ref="G5:G19" si="4">G4+1</f>
+        <f t="shared" ref="G5:G19" si="5">G4+1</f>
         <v>73</v>
       </c>
       <c r="H5" s="19">
         <v>26.5</v>
       </c>
       <c r="I5" s="23">
-        <f t="shared" ref="I5:I19" si="5">(1/H5)</f>
+        <f t="shared" ref="I5:I19" si="6">(1/H5)</f>
         <v>3.7735849056603772E-2</v>
       </c>
       <c r="J5" s="6">
-        <f t="shared" ref="J5:J19" si="6">D5/H5</f>
+        <f t="shared" ref="J5:J19" si="7">D5/H5</f>
         <v>41367.61449962265</v>
       </c>
       <c r="K5" s="6">
@@ -1845,7 +1857,7 @@
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6" s="21">
-        <f t="shared" ref="A6:A18" si="7">A5+1</f>
+        <f t="shared" ref="A6:A18" si="8">A5+1</f>
         <v>2028</v>
       </c>
       <c r="B6" s="6">
@@ -1855,7 +1867,7 @@
         <v>5000</v>
       </c>
       <c r="D6" s="6">
-        <f>D5+K5-J5-B5</f>
+        <f t="shared" si="4"/>
         <v>1131611.0946371774</v>
       </c>
       <c r="E6" s="6">
@@ -1867,18 +1879,18 @@
         <v>12291.852503110284</v>
       </c>
       <c r="G6" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>74</v>
       </c>
       <c r="H6" s="19">
         <v>25.5</v>
       </c>
       <c r="I6" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.9215686274509803E-2</v>
       </c>
       <c r="J6" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44376.905672046174</v>
       </c>
       <c r="K6" s="6">
@@ -1958,7 +1970,7 @@
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2029</v>
       </c>
       <c r="B7" s="6">
@@ -1968,7 +1980,7 @@
         <v>5000</v>
       </c>
       <c r="D7" s="6">
-        <f>D6+K6-J6-B6</f>
+        <f t="shared" si="4"/>
         <v>1166446.9655897338</v>
       </c>
       <c r="E7" s="6">
@@ -1980,18 +1992,18 @@
         <v>14199.09745052898</v>
       </c>
       <c r="G7" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>75</v>
       </c>
       <c r="H7" s="19">
         <v>24.6</v>
       </c>
       <c r="I7" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.065040650406504E-2</v>
       </c>
       <c r="J7" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>47416.543316655843</v>
       </c>
       <c r="K7" s="6">
@@ -2068,7 +2080,7 @@
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A8" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2030</v>
       </c>
       <c r="B8" s="6">
@@ -2078,7 +2090,7 @@
         <v>5000</v>
       </c>
       <c r="D8" s="6">
-        <f>D7+K7-J7-B7</f>
+        <f t="shared" si="4"/>
         <v>1200681.7098643593</v>
       </c>
       <c r="E8" s="6">
@@ -2090,18 +2102,18 @@
         <v>15172.284871050419</v>
       </c>
       <c r="G8" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>76</v>
       </c>
       <c r="H8" s="19">
         <v>23.7</v>
       </c>
       <c r="I8" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.2194092827004218E-2</v>
       </c>
       <c r="J8" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>50661.675521702928</v>
       </c>
       <c r="K8" s="6">
@@ -2178,7 +2190,7 @@
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A9" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2031</v>
       </c>
       <c r="B9" s="6">
@@ -2188,7 +2200,7 @@
         <v>5000</v>
       </c>
       <c r="D9" s="6">
-        <f>D8+K8-J8-B8</f>
+        <f t="shared" si="4"/>
         <v>1234067.7540331616</v>
       </c>
       <c r="E9" s="6">
@@ -2200,18 +2212,18 @@
         <v>16148.693012307993</v>
       </c>
       <c r="G9" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>77</v>
       </c>
       <c r="H9" s="19">
         <v>22.9</v>
       </c>
       <c r="I9" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.3668122270742363E-2</v>
       </c>
       <c r="J9" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>53889.421573500505</v>
       </c>
       <c r="K9" s="6">
@@ -2288,7 +2300,7 @@
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2032</v>
       </c>
       <c r="B10" s="6">
@@ -2298,7 +2310,7 @@
         <v>5000</v>
       </c>
       <c r="D10" s="6">
-        <f>D9+K9-J9-B9</f>
+        <f t="shared" si="4"/>
         <v>1266563.0752419822</v>
       </c>
       <c r="E10" s="6">
@@ -2310,18 +2322,18 @@
         <v>17232.226604757296</v>
       </c>
       <c r="G10" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>78</v>
       </c>
       <c r="H10" s="15">
         <v>22</v>
       </c>
       <c r="I10" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.5454545454545456E-2</v>
       </c>
       <c r="J10" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>57571.048874635555</v>
       </c>
       <c r="K10" s="6">
@@ -2398,7 +2410,7 @@
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2033</v>
       </c>
       <c r="B11" s="6">
@@ -2408,7 +2420,7 @@
         <v>6500</v>
       </c>
       <c r="D11" s="6">
-        <f>D10+K10-J10-B10</f>
+        <f t="shared" si="4"/>
         <v>1297651.4416342855</v>
       </c>
       <c r="E11" s="6">
@@ -2420,18 +2432,18 @@
         <v>18803.753870546745</v>
       </c>
       <c r="G11" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>79</v>
       </c>
       <c r="H11" s="19">
         <v>21.1</v>
       </c>
       <c r="I11" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.7393364928909949E-2</v>
       </c>
       <c r="J11" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>61500.068323899781</v>
       </c>
       <c r="K11" s="6">
@@ -2508,7 +2520,7 @@
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2034</v>
       </c>
       <c r="B12" s="6">
@@ -2518,7 +2530,7 @@
         <v>6000</v>
       </c>
       <c r="D12" s="6">
-        <f>D11+K11-J11-B11</f>
+        <f t="shared" si="4"/>
         <v>1326986.9742247858</v>
       </c>
       <c r="E12" s="6">
@@ -2530,18 +2542,18 @@
         <v>20005.001233484891</v>
       </c>
       <c r="G12" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>80</v>
       </c>
       <c r="H12" s="19">
         <v>20.2</v>
       </c>
       <c r="I12" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>4.9504950495049507E-2</v>
       </c>
       <c r="J12" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>65692.42446657356</v>
       </c>
       <c r="K12" s="6">
@@ -2618,7 +2630,7 @@
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2035</v>
       </c>
       <c r="B13" s="6">
@@ -2628,7 +2640,7 @@
         <v>5500</v>
       </c>
       <c r="D13" s="6">
-        <f>D12+K12-J12-B12</f>
+        <f t="shared" si="4"/>
         <v>1354183.6379539473</v>
       </c>
       <c r="E13" s="6">
@@ -2640,18 +2652,18 @@
         <v>21195.407908614121</v>
       </c>
       <c r="G13" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>81</v>
       </c>
       <c r="H13" s="19">
         <v>19.399999999999999</v>
       </c>
       <c r="I13" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.1546391752577324E-2</v>
       </c>
       <c r="J13" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>69803.280306904504</v>
       </c>
       <c r="K13" s="6">
@@ -2728,7 +2740,7 @@
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2036</v>
       </c>
       <c r="B14" s="6">
@@ -2738,7 +2750,7 @@
         <v>3500</v>
       </c>
       <c r="D14" s="6">
-        <f>D13+K13-J13-B13</f>
+        <f t="shared" si="4"/>
         <v>1379173.2123038191</v>
       </c>
       <c r="E14" s="6">
@@ -2750,18 +2762,18 @@
         <v>22187.396992481583</v>
       </c>
       <c r="G14" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>82</v>
       </c>
       <c r="H14" s="19">
         <v>18.5</v>
       </c>
       <c r="I14" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.4054054054054057E-2</v>
       </c>
       <c r="J14" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>74549.903367774008</v>
       </c>
       <c r="K14" s="6">
@@ -2838,7 +2850,7 @@
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A15" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2037</v>
       </c>
       <c r="B15" s="6">
@@ -2848,7 +2860,7 @@
         <v>4000</v>
       </c>
       <c r="D15" s="6">
-        <f>D14+K14-J14-B14</f>
+        <f t="shared" si="4"/>
         <v>1401165.4337973124</v>
       </c>
       <c r="E15" s="6">
@@ -2860,18 +2872,18 @@
         <v>23756.358991351244</v>
       </c>
       <c r="G15" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>83</v>
       </c>
       <c r="H15" s="19">
         <v>17.7</v>
       </c>
       <c r="I15" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.6497175141242938E-2</v>
       </c>
       <c r="J15" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>79161.888915102405</v>
       </c>
       <c r="K15" s="6">
@@ -2948,7 +2960,7 @@
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A16" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2038</v>
       </c>
       <c r="B16" s="6">
@@ -2958,7 +2970,7 @@
         <v>10000</v>
       </c>
       <c r="D16" s="6">
-        <f>D15+K15-J15-B15</f>
+        <f t="shared" si="4"/>
         <v>1420085.1252480219</v>
       </c>
       <c r="E16" s="6">
@@ -2970,18 +2982,18 @@
         <v>26836.104063095758</v>
       </c>
       <c r="G16" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>84</v>
       </c>
       <c r="H16" s="19">
         <v>16.8</v>
       </c>
       <c r="I16" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.9523809523809521E-2</v>
       </c>
       <c r="J16" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>84528.876502858446</v>
       </c>
       <c r="K16" s="6">
@@ -3061,7 +3073,7 @@
     </row>
     <row r="17" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A17" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2039</v>
       </c>
       <c r="B17" s="6">
@@ -3071,7 +3083,7 @@
         <v>10000</v>
       </c>
       <c r="D17" s="6">
-        <f>D16+K16-J16-B16</f>
+        <f t="shared" si="4"/>
         <v>1434962.2075125249</v>
       </c>
       <c r="E17" s="6">
@@ -3083,18 +3095,18 @@
         <v>28435.163415762239</v>
       </c>
       <c r="G17" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>85</v>
       </c>
       <c r="H17" s="15">
         <v>16</v>
       </c>
       <c r="I17" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.25E-2</v>
       </c>
       <c r="J17" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>89685.137969532807</v>
       </c>
       <c r="K17" s="6">
@@ -3174,7 +3186,7 @@
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A18" s="21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>2040</v>
       </c>
       <c r="B18" s="6">
@@ -3184,7 +3196,7 @@
         <v>10000</v>
       </c>
       <c r="D18" s="6">
-        <f>D17+K17-J17-B17</f>
+        <f t="shared" si="4"/>
         <v>1445724.4240688689</v>
       </c>
       <c r="E18" s="6">
@@ -3196,18 +3208,18 @@
         <v>30109.718758863681</v>
       </c>
       <c r="G18" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>86</v>
       </c>
       <c r="H18" s="19">
         <v>15.2</v>
       </c>
       <c r="I18" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.5789473684210523E-2</v>
       </c>
       <c r="J18" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>95113.448951899278</v>
       </c>
       <c r="K18" s="6">
@@ -3308,18 +3320,18 @@
         <v>31817.58268116543</v>
       </c>
       <c r="G19" s="22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>87</v>
       </c>
       <c r="H19" s="19">
         <v>14.4</v>
       </c>
       <c r="I19" s="23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.9444444444444448E-2</v>
       </c>
       <c r="J19" s="6">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>100636.67255567988</v>
       </c>
       <c r="K19" s="6">

</xml_diff>